<commit_message>
Comments, Excel sheet, Word Document
> New comments and revamped comments
> Excel sheet
> Marking schedule in word document
</commit_message>
<xml_diff>
--- a/testingLog (1).xlsx
+++ b/testingLog (1).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sbhsschool-my.sharepoint.com/personal/dgreenwood_sbhs_school_nz1/Documents/DTC-Curriculum/L3-DTC/3.7 &amp; 3.8 Programming/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brad\OneDrive - Southland Boys' High School\2019\L2DTC\Canvas\Programming 2019\L2-Programming\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CEC499CC-3C7D-4663-A9A9-D7D3D111FA44}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="65" documentId="8_{CEC499CC-3C7D-4663-A9A9-D7D3D111FA44}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{F8374E73-3B43-4E3C-BBD2-D0843F68C272}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{A4740EA8-4B8B-4BE0-B10F-2A8FE17358D6}"/>
+    <workbookView xWindow="16545" yWindow="8580" windowWidth="21600" windowHeight="11505" xr2:uid="{A4740EA8-4B8B-4BE0-B10F-2A8FE17358D6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="52">
   <si>
     <t>What is being tested</t>
   </si>
@@ -52,6 +52,141 @@
   </si>
   <si>
     <t>playerXpos decreases and player image moves left on canvas</t>
+  </si>
+  <si>
+    <t>Player moves left on canvas</t>
+  </si>
+  <si>
+    <t>moving right</t>
+  </si>
+  <si>
+    <t>Non-Valid username</t>
+  </si>
+  <si>
+    <t>no username</t>
+  </si>
+  <si>
+    <t>asked for username again</t>
+  </si>
+  <si>
+    <t>username prompt appears again</t>
+  </si>
+  <si>
+    <t>right arrow key</t>
+  </si>
+  <si>
+    <t>playerXpos increases and player image moves left on canvas</t>
+  </si>
+  <si>
+    <t>Player moves right on canvas</t>
+  </si>
+  <si>
+    <t>Valid username</t>
+  </si>
+  <si>
+    <t>username entered</t>
+  </si>
+  <si>
+    <t>prompt only appears once</t>
+  </si>
+  <si>
+    <t>loser screen</t>
+  </si>
+  <si>
+    <t>winner screen</t>
+  </si>
+  <si>
+    <t>lose all lives</t>
+  </si>
+  <si>
+    <t>survive 15 seconds</t>
+  </si>
+  <si>
+    <t>winner screen appears</t>
+  </si>
+  <si>
+    <t>loser screen appears</t>
+  </si>
+  <si>
+    <t>Easy mode</t>
+  </si>
+  <si>
+    <t>Medium mode</t>
+  </si>
+  <si>
+    <t>Hard mode</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>Least lives and least jellyfish</t>
+  </si>
+  <si>
+    <t>Most lives and Most jellyfish</t>
+  </si>
+  <si>
+    <t>Middle amount of lives and middle amount of jellyfish</t>
+  </si>
+  <si>
+    <t>Collosions</t>
+  </si>
+  <si>
+    <t>Lives</t>
+  </si>
+  <si>
+    <t>Time to beat</t>
+  </si>
+  <si>
+    <t>Player gets struck by enemy (jellyfish)</t>
+  </si>
+  <si>
+    <t>Lives get to 0</t>
+  </si>
+  <si>
+    <t>survive the time to beat</t>
+  </si>
+  <si>
+    <t>Lives go down</t>
+  </si>
+  <si>
+    <t>Game stops and loser screen appears</t>
+  </si>
+  <si>
+    <t>The winner screen appear after time to survive</t>
+  </si>
+  <si>
+    <t>Player boundarys</t>
+  </si>
+  <si>
+    <t>Player hits wall</t>
+  </si>
+  <si>
+    <t>Player cannot progress further in that direction</t>
+  </si>
+  <si>
+    <t>Wrong number (difficulty)</t>
+  </si>
+  <si>
+    <t>Any other number than 1, 2 or 3</t>
+  </si>
+  <si>
+    <t>Nothing happens</t>
+  </si>
+  <si>
+    <t>cancel button or nothing in propmt</t>
+  </si>
+  <si>
+    <t>Cancel or nothing in prompt</t>
+  </si>
+  <si>
+    <t>Prompt reappears</t>
   </si>
 </sst>
 </file>
@@ -452,7 +587,7 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -487,91 +622,205 @@
       <c r="C2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="4"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
+      <c r="D2" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="33" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
+      <c r="A4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
+      <c r="A5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
+      <c r="A6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
+      <c r="A7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
+      <c r="A8" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="33" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
+      <c r="A10" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="33" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
+      <c r="A12" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
+      <c r="A13" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
+      <c r="A14" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="33" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="33" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
@@ -616,6 +865,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <ReferenceId xmlns="d11f87b1-ee25-42cc-a142-7e0050601da8">14434952-8f46-424a-86b4-8246224ab183</ReferenceId>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100EF57B91C2D6BAB4EAB22BC3D656199D1" ma:contentTypeVersion="3" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bdcae8afadbfa03c8651d567f9e3a326">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="d11f87b1-ee25-42cc-a142-7e0050601da8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="298e1f1d6d31af662d0e3f709724dc2d" ns2:_="">
     <xsd:import namespace="d11f87b1-ee25-42cc-a142-7e0050601da8"/>
@@ -753,36 +1019,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <ReferenceId xmlns="d11f87b1-ee25-42cc-a142-7e0050601da8">14434952-8f46-424a-86b4-8246224ab183</ReferenceId>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C41F9991-9720-4EB2-907A-4EA30723FFA3}"/>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E60CF964-E5B0-4456-94C9-62848076981E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{49705E9F-1DBC-44ED-AB34-BAD166CF391C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="2e3d35ac-3642-4169-bdb3-94441f3ce34f"/>
@@ -795,6 +1032,33 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="d11f87b1-ee25-42cc-a142-7e0050601da8"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E60CF964-E5B0-4456-94C9-62848076981E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C41F9991-9720-4EB2-907A-4EA30723FFA3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="d11f87b1-ee25-42cc-a142-7e0050601da8"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>